<commit_message>
add dry density and use dynamic porosity to calculate VMC
</commit_message>
<xml_diff>
--- a/stanwell/data/manual/manual.xlsx
+++ b/stanwell/data/manual/manual.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20342"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20358"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\stanwell\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\UQ_PhD Study\projects\stanwell\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34BE8361-5C05-4031-AA97-F71057DC0A7E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{761F6BB8-8BED-431F-8128-77AAE8061FFD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19140" windowHeight="18915" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -833,10 +833,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B341"/>
+  <dimension ref="A1:B757"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B263" sqref="B263"/>
+    <sheetView tabSelected="1" topLeftCell="A726" workbookViewId="0">
+      <selection activeCell="B606" sqref="B606"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3573,6 +3573,3334 @@
         <v>169</v>
       </c>
     </row>
+    <row r="342" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A342" s="1">
+        <v>43526.5</v>
+      </c>
+      <c r="B342">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="343" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A343" s="1">
+        <v>43527.5</v>
+      </c>
+      <c r="B343">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="344" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A344" s="1">
+        <v>43528.5</v>
+      </c>
+      <c r="B344">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="345" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A345" s="1">
+        <v>43529.5</v>
+      </c>
+      <c r="B345">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="346" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A346" s="1">
+        <v>43530.5</v>
+      </c>
+      <c r="B346">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="347" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A347" s="1">
+        <v>43531.5</v>
+      </c>
+      <c r="B347">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="348" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A348" s="1">
+        <v>43532.5</v>
+      </c>
+      <c r="B348">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="349" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A349" s="1">
+        <v>43533.5</v>
+      </c>
+      <c r="B349">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="350" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A350" s="1">
+        <v>43534.5</v>
+      </c>
+      <c r="B350">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="351" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A351" s="1">
+        <v>43535.5</v>
+      </c>
+      <c r="B351">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="352" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A352" s="1">
+        <v>43536.5</v>
+      </c>
+      <c r="B352">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="353" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A353" s="1">
+        <v>43537.5</v>
+      </c>
+      <c r="B353">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="354" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A354" s="1">
+        <v>43538.5</v>
+      </c>
+      <c r="B354">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="355" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A355" s="1">
+        <v>43539.5</v>
+      </c>
+      <c r="B355">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="356" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A356" s="1">
+        <v>43540.5</v>
+      </c>
+      <c r="B356">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="357" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A357" s="1">
+        <v>43541.5</v>
+      </c>
+      <c r="B357">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="358" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A358" s="1">
+        <v>43542.5</v>
+      </c>
+      <c r="B358">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="359" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A359" s="1">
+        <v>43543.5</v>
+      </c>
+      <c r="B359">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="360" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A360" s="1">
+        <v>43544.5</v>
+      </c>
+      <c r="B360">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="361" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A361" s="1">
+        <v>43545.5</v>
+      </c>
+      <c r="B361">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="362" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A362" s="1">
+        <v>43546.5</v>
+      </c>
+      <c r="B362">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="363" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A363" s="1">
+        <v>43547.5</v>
+      </c>
+      <c r="B363">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="364" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A364" s="1">
+        <v>43548.5</v>
+      </c>
+      <c r="B364">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="365" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A365" s="1">
+        <v>43549.5</v>
+      </c>
+      <c r="B365">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="366" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A366" s="1">
+        <v>43550.5</v>
+      </c>
+      <c r="B366">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="367" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A367" s="1">
+        <v>43551.5</v>
+      </c>
+      <c r="B367">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="368" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A368" s="1">
+        <v>43552.5</v>
+      </c>
+      <c r="B368">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="369" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A369" s="1">
+        <v>43553.5</v>
+      </c>
+      <c r="B369">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="370" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A370" s="1">
+        <v>43554.5</v>
+      </c>
+      <c r="B370">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="371" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A371" s="1">
+        <v>43555.5</v>
+      </c>
+      <c r="B371">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="372" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A372" s="1">
+        <v>43556.5</v>
+      </c>
+      <c r="B372">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="373" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A373" s="1">
+        <v>43557.5</v>
+      </c>
+      <c r="B373">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="374" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A374" s="1">
+        <v>43558.5</v>
+      </c>
+      <c r="B374">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="375" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A375" s="1">
+        <v>43559.5</v>
+      </c>
+      <c r="B375">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="376" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A376" s="1">
+        <v>43560.5</v>
+      </c>
+      <c r="B376">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="377" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A377" s="1">
+        <v>43561.5</v>
+      </c>
+      <c r="B377">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="378" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A378" s="1">
+        <v>43562.5</v>
+      </c>
+      <c r="B378">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="379" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A379" s="1">
+        <v>43563.5</v>
+      </c>
+      <c r="B379">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="380" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A380" s="1">
+        <v>43564.5</v>
+      </c>
+      <c r="B380">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="381" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A381" s="1">
+        <v>43565.5</v>
+      </c>
+      <c r="B381">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="382" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A382" s="1">
+        <v>43566.5</v>
+      </c>
+      <c r="B382">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="383" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A383" s="1">
+        <v>43567.5</v>
+      </c>
+      <c r="B383">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="384" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A384" s="1">
+        <v>43568.5</v>
+      </c>
+      <c r="B384">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="385" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A385" s="1">
+        <v>43569.5</v>
+      </c>
+      <c r="B385">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="386" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A386" s="1">
+        <v>43570.5</v>
+      </c>
+      <c r="B386">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="387" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A387" s="1">
+        <v>43571.5</v>
+      </c>
+      <c r="B387">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="388" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A388" s="1">
+        <v>43572.5</v>
+      </c>
+      <c r="B388">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="389" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A389" s="1">
+        <v>43573.5</v>
+      </c>
+      <c r="B389">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="390" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A390" s="1">
+        <v>43574.5</v>
+      </c>
+      <c r="B390">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="391" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A391" s="1">
+        <v>43575.5</v>
+      </c>
+      <c r="B391">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="392" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A392" s="1">
+        <v>43576.5</v>
+      </c>
+      <c r="B392">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="393" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A393" s="1">
+        <v>43577.5</v>
+      </c>
+      <c r="B393">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="394" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A394" s="1">
+        <v>43578.5</v>
+      </c>
+      <c r="B394">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="395" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A395" s="1">
+        <v>43579.5</v>
+      </c>
+      <c r="B395">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="396" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A396" s="1">
+        <v>43580.5</v>
+      </c>
+      <c r="B396">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="397" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A397" s="1">
+        <v>43581.5</v>
+      </c>
+      <c r="B397">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="398" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A398" s="1">
+        <v>43582.5</v>
+      </c>
+      <c r="B398">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="399" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A399" s="1">
+        <v>43583.5</v>
+      </c>
+      <c r="B399">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="400" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A400" s="1">
+        <v>43584.5</v>
+      </c>
+      <c r="B400">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="401" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A401" s="1">
+        <v>43585.5</v>
+      </c>
+      <c r="B401">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="402" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A402" s="1">
+        <v>43586.5</v>
+      </c>
+      <c r="B402">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="403" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A403" s="1">
+        <v>43587.5</v>
+      </c>
+      <c r="B403">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="404" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A404" s="1">
+        <v>43588.5</v>
+      </c>
+      <c r="B404">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="405" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A405" s="1">
+        <v>43589.5</v>
+      </c>
+      <c r="B405">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="406" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A406" s="1">
+        <v>43590.5</v>
+      </c>
+      <c r="B406">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="407" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A407" s="1">
+        <v>43591.5</v>
+      </c>
+      <c r="B407">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="408" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A408" s="1">
+        <v>43592.5</v>
+      </c>
+      <c r="B408">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="409" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A409" s="1">
+        <v>43593.5</v>
+      </c>
+      <c r="B409">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="410" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A410" s="1">
+        <v>43594.5</v>
+      </c>
+      <c r="B410">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="411" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A411" s="1">
+        <v>43595.5</v>
+      </c>
+      <c r="B411">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="412" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A412" s="1">
+        <v>43596.5</v>
+      </c>
+      <c r="B412">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="413" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A413" s="1">
+        <v>43597.5</v>
+      </c>
+      <c r="B413">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="414" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A414" s="1">
+        <v>43598.5</v>
+      </c>
+      <c r="B414">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="415" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A415" s="1">
+        <v>43599.5</v>
+      </c>
+      <c r="B415">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="416" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A416" s="1">
+        <v>43600.5</v>
+      </c>
+      <c r="B416">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="417" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A417" s="1">
+        <v>43601.5</v>
+      </c>
+      <c r="B417">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="418" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A418" s="1">
+        <v>43602.5</v>
+      </c>
+      <c r="B418">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="419" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A419" s="1">
+        <v>43603.5</v>
+      </c>
+      <c r="B419">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="420" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A420" s="1">
+        <v>43604.5</v>
+      </c>
+      <c r="B420">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="421" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A421" s="1">
+        <v>43605.5</v>
+      </c>
+      <c r="B421">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="422" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A422" s="1">
+        <v>43606.5</v>
+      </c>
+      <c r="B422">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="423" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A423" s="1">
+        <v>43607.5</v>
+      </c>
+      <c r="B423">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="424" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A424" s="1">
+        <v>43608.5</v>
+      </c>
+      <c r="B424">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="425" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A425" s="1">
+        <v>43609.5</v>
+      </c>
+      <c r="B425">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="426" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A426" s="1">
+        <v>43610.5</v>
+      </c>
+      <c r="B426">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="427" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A427" s="1">
+        <v>43611.5</v>
+      </c>
+      <c r="B427">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="428" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A428" s="1">
+        <v>43612.5</v>
+      </c>
+      <c r="B428">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="429" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A429" s="1">
+        <v>43613.5</v>
+      </c>
+      <c r="B429">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="430" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A430" s="1">
+        <v>43614.5</v>
+      </c>
+      <c r="B430">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="431" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A431" s="1">
+        <v>43615.5</v>
+      </c>
+      <c r="B431">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="432" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A432" s="1">
+        <v>43616.5</v>
+      </c>
+      <c r="B432">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="433" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A433" s="1">
+        <v>43617.5</v>
+      </c>
+      <c r="B433">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="434" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A434" s="1">
+        <v>43618.5</v>
+      </c>
+      <c r="B434">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="435" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A435" s="1">
+        <v>43619.5</v>
+      </c>
+      <c r="B435">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="436" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A436" s="1">
+        <v>43620.5</v>
+      </c>
+      <c r="B436">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="437" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A437" s="1">
+        <v>43621.5</v>
+      </c>
+      <c r="B437">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="438" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A438" s="1">
+        <v>43622.5</v>
+      </c>
+      <c r="B438">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="439" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A439" s="1">
+        <v>43623.5</v>
+      </c>
+      <c r="B439">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="440" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A440" s="1">
+        <v>43624.5</v>
+      </c>
+      <c r="B440">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="441" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A441" s="1">
+        <v>43625.5</v>
+      </c>
+      <c r="B441">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="442" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A442" s="1">
+        <v>43626.5</v>
+      </c>
+      <c r="B442">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="443" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A443" s="1">
+        <v>43627.5</v>
+      </c>
+      <c r="B443">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="444" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A444" s="1">
+        <v>43628.5</v>
+      </c>
+      <c r="B444">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="445" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A445" s="1">
+        <v>43629.5</v>
+      </c>
+      <c r="B445">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="446" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A446" s="1">
+        <v>43630.5</v>
+      </c>
+      <c r="B446">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="447" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A447" s="1">
+        <v>43631.5</v>
+      </c>
+      <c r="B447">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="448" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A448" s="1">
+        <v>43632.5</v>
+      </c>
+      <c r="B448">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="449" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A449" s="1">
+        <v>43633.5</v>
+      </c>
+      <c r="B449">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="450" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A450" s="1">
+        <v>43634.5</v>
+      </c>
+      <c r="B450">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="451" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A451" s="1">
+        <v>43635.5</v>
+      </c>
+      <c r="B451">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="452" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A452" s="1">
+        <v>43636.5</v>
+      </c>
+      <c r="B452">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="453" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A453" s="1">
+        <v>43637.5</v>
+      </c>
+      <c r="B453">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="454" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A454" s="1">
+        <v>43638.5</v>
+      </c>
+      <c r="B454">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="455" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A455" s="1">
+        <v>43639.5</v>
+      </c>
+      <c r="B455">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="456" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A456" s="1">
+        <v>43640.5</v>
+      </c>
+      <c r="B456">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="457" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A457" s="1">
+        <v>43641.5</v>
+      </c>
+      <c r="B457">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="458" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A458" s="1">
+        <v>43642.5</v>
+      </c>
+      <c r="B458">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="459" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A459" s="1">
+        <v>43643.5</v>
+      </c>
+      <c r="B459">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="460" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A460" s="1">
+        <v>43644.5</v>
+      </c>
+      <c r="B460">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="461" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A461" s="1">
+        <v>43645.5</v>
+      </c>
+      <c r="B461">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="462" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A462" s="1">
+        <v>43646.5</v>
+      </c>
+      <c r="B462">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="463" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A463" s="1">
+        <v>43647.5</v>
+      </c>
+      <c r="B463">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="464" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A464" s="1">
+        <v>43648.5</v>
+      </c>
+      <c r="B464">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="465" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A465" s="1">
+        <v>43649.5</v>
+      </c>
+      <c r="B465">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="466" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A466" s="1">
+        <v>43650.5</v>
+      </c>
+      <c r="B466">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="467" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A467" s="1">
+        <v>43651.5</v>
+      </c>
+      <c r="B467">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="468" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A468" s="1">
+        <v>43652.5</v>
+      </c>
+      <c r="B468">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="469" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A469" s="1">
+        <v>43653.5</v>
+      </c>
+      <c r="B469">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="470" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A470" s="1">
+        <v>43654.5</v>
+      </c>
+      <c r="B470">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="471" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A471" s="1">
+        <v>43655.5</v>
+      </c>
+      <c r="B471">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="472" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A472" s="1">
+        <v>43656.5</v>
+      </c>
+      <c r="B472">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="473" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A473" s="1">
+        <v>43657.5</v>
+      </c>
+      <c r="B473">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="474" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A474" s="1">
+        <v>43658.5</v>
+      </c>
+      <c r="B474">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="475" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A475" s="1">
+        <v>43659.5</v>
+      </c>
+      <c r="B475">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="476" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A476" s="1">
+        <v>43660.5</v>
+      </c>
+      <c r="B476">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="477" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A477" s="1">
+        <v>43661.5</v>
+      </c>
+      <c r="B477">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="478" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A478" s="1">
+        <v>43662.5</v>
+      </c>
+      <c r="B478">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="479" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A479" s="1">
+        <v>43663.5</v>
+      </c>
+      <c r="B479">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="480" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A480" s="1">
+        <v>43664.5</v>
+      </c>
+      <c r="B480">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="481" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A481" s="1">
+        <v>43665.5</v>
+      </c>
+      <c r="B481">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="482" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A482" s="1">
+        <v>43666.5</v>
+      </c>
+      <c r="B482">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="483" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A483" s="1">
+        <v>43667.5</v>
+      </c>
+      <c r="B483">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="484" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A484" s="1">
+        <v>43668.5</v>
+      </c>
+      <c r="B484">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="485" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A485" s="1">
+        <v>43669.5</v>
+      </c>
+      <c r="B485">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="486" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A486" s="1">
+        <v>43670.5</v>
+      </c>
+      <c r="B486">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="487" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A487" s="1">
+        <v>43671.5</v>
+      </c>
+      <c r="B487">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="488" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A488" s="1">
+        <v>43672.5</v>
+      </c>
+      <c r="B488">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="489" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A489" s="1">
+        <v>43673.5</v>
+      </c>
+      <c r="B489">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="490" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A490" s="1">
+        <v>43674.5</v>
+      </c>
+      <c r="B490">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="491" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A491" s="1">
+        <v>43675.5</v>
+      </c>
+      <c r="B491">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="492" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A492" s="1">
+        <v>43676.5</v>
+      </c>
+      <c r="B492">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="493" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A493" s="1">
+        <v>43677.5</v>
+      </c>
+      <c r="B493">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="494" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A494" s="1">
+        <v>43678.5</v>
+      </c>
+      <c r="B494">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="495" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A495" s="1">
+        <v>43679.5</v>
+      </c>
+      <c r="B495">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="496" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A496" s="1">
+        <v>43680.5</v>
+      </c>
+      <c r="B496">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="497" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A497" s="1">
+        <v>43681.5</v>
+      </c>
+      <c r="B497">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="498" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A498" s="1">
+        <v>43682.5</v>
+      </c>
+      <c r="B498">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="499" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A499" s="1">
+        <v>43683.5</v>
+      </c>
+      <c r="B499">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="500" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A500" s="1">
+        <v>43684.5</v>
+      </c>
+      <c r="B500">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="501" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A501" s="1">
+        <v>43685.5</v>
+      </c>
+      <c r="B501">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="502" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A502" s="1">
+        <v>43686.5</v>
+      </c>
+      <c r="B502">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="503" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A503" s="1">
+        <v>43687.5</v>
+      </c>
+      <c r="B503">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="504" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A504" s="1">
+        <v>43688.5</v>
+      </c>
+      <c r="B504">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="505" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A505" s="1">
+        <v>43689.5</v>
+      </c>
+      <c r="B505">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="506" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A506" s="1">
+        <v>43690.5</v>
+      </c>
+      <c r="B506">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="507" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A507" s="1">
+        <v>43691.5</v>
+      </c>
+      <c r="B507">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="508" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A508" s="1">
+        <v>43692.5</v>
+      </c>
+      <c r="B508">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="509" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A509" s="1">
+        <v>43693.5</v>
+      </c>
+      <c r="B509">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="510" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A510" s="1">
+        <v>43694.5</v>
+      </c>
+      <c r="B510">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="511" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A511" s="1">
+        <v>43695.5</v>
+      </c>
+      <c r="B511">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="512" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A512" s="1">
+        <v>43696.5</v>
+      </c>
+      <c r="B512">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="513" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A513" s="1">
+        <v>43697.5</v>
+      </c>
+      <c r="B513">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="514" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A514" s="1">
+        <v>43698.5</v>
+      </c>
+      <c r="B514">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="515" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A515" s="1">
+        <v>43699.5</v>
+      </c>
+      <c r="B515">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="516" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A516" s="1">
+        <v>43700.5</v>
+      </c>
+      <c r="B516">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="517" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A517" s="1">
+        <v>43701.5</v>
+      </c>
+      <c r="B517">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="518" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A518" s="1">
+        <v>43702.5</v>
+      </c>
+      <c r="B518">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="519" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A519" s="1">
+        <v>43703.5</v>
+      </c>
+      <c r="B519">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="520" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A520" s="1">
+        <v>43704.5</v>
+      </c>
+      <c r="B520">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="521" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A521" s="1">
+        <v>43705.5</v>
+      </c>
+      <c r="B521">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="522" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A522" s="1">
+        <v>43706.5</v>
+      </c>
+      <c r="B522">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="523" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A523" s="1">
+        <v>43707.5</v>
+      </c>
+      <c r="B523">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="524" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A524" s="1">
+        <v>43708.5</v>
+      </c>
+      <c r="B524">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="525" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A525" s="1">
+        <v>43709.5</v>
+      </c>
+      <c r="B525">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="526" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A526" s="1">
+        <v>43710.5</v>
+      </c>
+      <c r="B526">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="527" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A527" s="1">
+        <v>43711.5</v>
+      </c>
+      <c r="B527">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="528" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A528" s="1">
+        <v>43712.5</v>
+      </c>
+      <c r="B528">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="529" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A529" s="1">
+        <v>43713.5</v>
+      </c>
+      <c r="B529">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="530" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A530" s="1">
+        <v>43714.5</v>
+      </c>
+      <c r="B530">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="531" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A531" s="1">
+        <v>43715.5</v>
+      </c>
+      <c r="B531">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="532" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A532" s="1">
+        <v>43716.5</v>
+      </c>
+      <c r="B532">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="533" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A533" s="1">
+        <v>43717.5</v>
+      </c>
+      <c r="B533">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="534" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A534" s="1">
+        <v>43718.5</v>
+      </c>
+      <c r="B534">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="535" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A535" s="1">
+        <v>43719.5</v>
+      </c>
+      <c r="B535">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="536" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A536" s="1">
+        <v>43720.5</v>
+      </c>
+      <c r="B536">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="537" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A537" s="1">
+        <v>43721.5</v>
+      </c>
+      <c r="B537">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="538" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A538" s="1">
+        <v>43722.5</v>
+      </c>
+      <c r="B538">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="539" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A539" s="1">
+        <v>43723.5</v>
+      </c>
+      <c r="B539">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="540" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A540" s="1">
+        <v>43724.5</v>
+      </c>
+      <c r="B540">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="541" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A541" s="1">
+        <v>43725.5</v>
+      </c>
+      <c r="B541">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="542" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A542" s="1">
+        <v>43726.5</v>
+      </c>
+      <c r="B542">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="543" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A543" s="1">
+        <v>43727.5</v>
+      </c>
+      <c r="B543">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="544" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A544" s="1">
+        <v>43728.5</v>
+      </c>
+      <c r="B544">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="545" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A545" s="1">
+        <v>43729.5</v>
+      </c>
+      <c r="B545">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="546" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A546" s="1">
+        <v>43730.5</v>
+      </c>
+      <c r="B546">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="547" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A547" s="1">
+        <v>43731.5</v>
+      </c>
+      <c r="B547">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="548" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A548" s="1">
+        <v>43732.5</v>
+      </c>
+      <c r="B548">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="549" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A549" s="1">
+        <v>43733.5</v>
+      </c>
+      <c r="B549">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="550" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A550" s="1">
+        <v>43734.5</v>
+      </c>
+      <c r="B550">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="551" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A551" s="1">
+        <v>43735.5</v>
+      </c>
+      <c r="B551">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="552" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A552" s="1">
+        <v>43736.5</v>
+      </c>
+      <c r="B552">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="553" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A553" s="1">
+        <v>43737.5</v>
+      </c>
+      <c r="B553">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="554" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A554" s="1">
+        <v>43738.5</v>
+      </c>
+      <c r="B554">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="555" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A555" s="1">
+        <v>43739.5</v>
+      </c>
+      <c r="B555">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="556" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A556" s="1">
+        <v>43740.5</v>
+      </c>
+      <c r="B556">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="557" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A557" s="1">
+        <v>43741.5</v>
+      </c>
+      <c r="B557">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="558" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A558" s="1">
+        <v>43742.5</v>
+      </c>
+      <c r="B558">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="559" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A559" s="1">
+        <v>43743.5</v>
+      </c>
+      <c r="B559">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="560" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A560" s="1">
+        <v>43744.5</v>
+      </c>
+      <c r="B560">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="561" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A561" s="1">
+        <v>43745.5</v>
+      </c>
+      <c r="B561">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="562" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A562" s="1">
+        <v>43746.5</v>
+      </c>
+      <c r="B562">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="563" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A563" s="1">
+        <v>43747.5</v>
+      </c>
+      <c r="B563">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="564" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A564" s="1">
+        <v>43748.5</v>
+      </c>
+      <c r="B564">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="565" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A565" s="1">
+        <v>43749.5</v>
+      </c>
+      <c r="B565">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="566" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A566" s="1">
+        <v>43750.5</v>
+      </c>
+      <c r="B566">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="567" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A567" s="1">
+        <v>43751.5</v>
+      </c>
+      <c r="B567">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="568" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A568" s="1">
+        <v>43752.5</v>
+      </c>
+      <c r="B568">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="569" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A569" s="1">
+        <v>43753.5</v>
+      </c>
+      <c r="B569">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="570" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A570" s="1">
+        <v>43754.5</v>
+      </c>
+      <c r="B570">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="571" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A571" s="1">
+        <v>43755.5</v>
+      </c>
+      <c r="B571">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="572" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A572" s="1">
+        <v>43756.5</v>
+      </c>
+      <c r="B572">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="573" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A573" s="1">
+        <v>43757.5</v>
+      </c>
+      <c r="B573">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="574" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A574" s="1">
+        <v>43758.5</v>
+      </c>
+      <c r="B574">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="575" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A575" s="1">
+        <v>43759.5</v>
+      </c>
+      <c r="B575">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="576" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A576" s="1">
+        <v>43760.5</v>
+      </c>
+      <c r="B576">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="577" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A577" s="1">
+        <v>43761.5</v>
+      </c>
+      <c r="B577">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="578" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A578" s="1">
+        <v>43762.5</v>
+      </c>
+      <c r="B578">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="579" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A579" s="1">
+        <v>43763.5</v>
+      </c>
+      <c r="B579">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="580" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A580" s="1">
+        <v>43764.5</v>
+      </c>
+      <c r="B580">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="581" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A581" s="1">
+        <v>43765.5</v>
+      </c>
+      <c r="B581">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="582" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A582" s="1">
+        <v>43766.5</v>
+      </c>
+      <c r="B582">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="583" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A583" s="1">
+        <v>43767.5</v>
+      </c>
+      <c r="B583">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="584" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A584" s="1">
+        <v>43768.5</v>
+      </c>
+      <c r="B584">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="585" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A585" s="1">
+        <v>43769.5</v>
+      </c>
+      <c r="B585">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="586" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A586" s="1">
+        <v>43770.5</v>
+      </c>
+      <c r="B586">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="587" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A587" s="1">
+        <v>43771.5</v>
+      </c>
+      <c r="B587">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="588" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A588" s="1">
+        <v>43772.5</v>
+      </c>
+      <c r="B588">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="589" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A589" s="1">
+        <v>43773.5</v>
+      </c>
+      <c r="B589">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="590" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A590" s="1">
+        <v>43774.5</v>
+      </c>
+      <c r="B590">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="591" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A591" s="1">
+        <v>43775.5</v>
+      </c>
+      <c r="B591">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="592" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A592" s="1">
+        <v>43776.5</v>
+      </c>
+      <c r="B592">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="593" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A593" s="1">
+        <v>43777.5</v>
+      </c>
+      <c r="B593">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="594" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A594" s="1">
+        <v>43778.5</v>
+      </c>
+      <c r="B594">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="595" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A595" s="1">
+        <v>43779.5</v>
+      </c>
+      <c r="B595">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="596" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A596" s="1">
+        <v>43780.5</v>
+      </c>
+      <c r="B596">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="597" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A597" s="1">
+        <v>43781.5</v>
+      </c>
+      <c r="B597">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="598" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A598" s="1">
+        <v>43782.5</v>
+      </c>
+      <c r="B598">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="599" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A599" s="1">
+        <v>43783.5</v>
+      </c>
+      <c r="B599">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="600" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A600" s="1">
+        <v>43784.5</v>
+      </c>
+      <c r="B600">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="601" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A601" s="1">
+        <v>43785.5</v>
+      </c>
+      <c r="B601">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="602" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A602" s="1">
+        <v>43786.5</v>
+      </c>
+      <c r="B602">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="603" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A603" s="1">
+        <v>43787.5</v>
+      </c>
+      <c r="B603">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="604" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A604" s="1">
+        <v>43788.5</v>
+      </c>
+      <c r="B604">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="605" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A605" s="1">
+        <v>43789.5</v>
+      </c>
+      <c r="B605">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="606" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A606" s="1">
+        <v>43790.5</v>
+      </c>
+      <c r="B606">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="607" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A607" s="1">
+        <v>43791.5</v>
+      </c>
+      <c r="B607">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="608" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A608" s="1">
+        <v>43792.5</v>
+      </c>
+      <c r="B608">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="609" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A609" s="1">
+        <v>43793.5</v>
+      </c>
+      <c r="B609">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="610" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A610" s="1">
+        <v>43794.5</v>
+      </c>
+      <c r="B610">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="611" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A611" s="1">
+        <v>43795.5</v>
+      </c>
+      <c r="B611">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="612" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A612" s="1">
+        <v>43796.5</v>
+      </c>
+      <c r="B612">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="613" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A613" s="1">
+        <v>43797.5</v>
+      </c>
+      <c r="B613">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="614" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A614" s="1">
+        <v>43798.5</v>
+      </c>
+      <c r="B614">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="615" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A615" s="1">
+        <v>43799.5</v>
+      </c>
+      <c r="B615">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="616" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A616" s="1">
+        <v>43800.5</v>
+      </c>
+      <c r="B616">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="617" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A617" s="1">
+        <v>43801.5</v>
+      </c>
+      <c r="B617">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="618" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A618" s="1">
+        <v>43802.5</v>
+      </c>
+      <c r="B618">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="619" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A619" s="1">
+        <v>43803.5</v>
+      </c>
+      <c r="B619">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="620" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A620" s="1">
+        <v>43804.5</v>
+      </c>
+      <c r="B620">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="621" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A621" s="1">
+        <v>43805.5</v>
+      </c>
+      <c r="B621">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="622" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A622" s="1">
+        <v>43806.5</v>
+      </c>
+      <c r="B622">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="623" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A623" s="1">
+        <v>43807.5</v>
+      </c>
+      <c r="B623">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="624" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A624" s="1">
+        <v>43808.5</v>
+      </c>
+      <c r="B624">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="625" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A625" s="1">
+        <v>43809.5</v>
+      </c>
+      <c r="B625">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="626" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A626" s="1">
+        <v>43810.5</v>
+      </c>
+      <c r="B626">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="627" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A627" s="1">
+        <v>43811.5</v>
+      </c>
+      <c r="B627">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="628" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A628" s="1">
+        <v>43812.5</v>
+      </c>
+      <c r="B628">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="629" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A629" s="1">
+        <v>43813.5</v>
+      </c>
+      <c r="B629">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="630" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A630" s="1">
+        <v>43814.5</v>
+      </c>
+      <c r="B630">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="631" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A631" s="1">
+        <v>43815.5</v>
+      </c>
+      <c r="B631">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="632" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A632" s="1">
+        <v>43816.5</v>
+      </c>
+      <c r="B632">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="633" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A633" s="1">
+        <v>43817.5</v>
+      </c>
+      <c r="B633">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="634" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A634" s="1">
+        <v>43818.5</v>
+      </c>
+      <c r="B634">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="635" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A635" s="1">
+        <v>43819.5</v>
+      </c>
+      <c r="B635">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="636" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A636" s="1">
+        <v>43820.5</v>
+      </c>
+      <c r="B636">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="637" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A637" s="1">
+        <v>43821.5</v>
+      </c>
+      <c r="B637">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="638" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A638" s="1">
+        <v>43822.5</v>
+      </c>
+      <c r="B638">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="639" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A639" s="1">
+        <v>43823.5</v>
+      </c>
+      <c r="B639">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="640" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A640" s="1">
+        <v>43824.5</v>
+      </c>
+      <c r="B640">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="641" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A641" s="1">
+        <v>43825.5</v>
+      </c>
+      <c r="B641">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="642" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A642" s="1">
+        <v>43826.5</v>
+      </c>
+      <c r="B642">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="643" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A643" s="1">
+        <v>43827.5</v>
+      </c>
+      <c r="B643">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="644" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A644" s="1">
+        <v>43828.5</v>
+      </c>
+      <c r="B644">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="645" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A645" s="1">
+        <v>43829.5</v>
+      </c>
+      <c r="B645">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="646" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A646" s="1">
+        <v>43830.5</v>
+      </c>
+      <c r="B646">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="647" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A647" s="1">
+        <v>43831.5</v>
+      </c>
+      <c r="B647">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="648" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A648" s="1">
+        <v>43832.5</v>
+      </c>
+      <c r="B648">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="649" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A649" s="1">
+        <v>43833.5</v>
+      </c>
+      <c r="B649">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="650" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A650" s="1">
+        <v>43834.5</v>
+      </c>
+      <c r="B650">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="651" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A651" s="1">
+        <v>43835.5</v>
+      </c>
+      <c r="B651">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="652" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A652" s="1">
+        <v>43836.5</v>
+      </c>
+      <c r="B652">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="653" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A653" s="1">
+        <v>43837.5</v>
+      </c>
+      <c r="B653">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="654" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A654" s="1">
+        <v>43838.5</v>
+      </c>
+      <c r="B654">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="655" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A655" s="1">
+        <v>43839.5</v>
+      </c>
+      <c r="B655">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="656" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A656" s="1">
+        <v>43840.5</v>
+      </c>
+      <c r="B656">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="657" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A657" s="1">
+        <v>43841.5</v>
+      </c>
+      <c r="B657">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="658" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A658" s="1">
+        <v>43842.5</v>
+      </c>
+      <c r="B658">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="659" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A659" s="1">
+        <v>43843.5</v>
+      </c>
+      <c r="B659">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="660" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A660" s="1">
+        <v>43844.5</v>
+      </c>
+      <c r="B660">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="661" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A661" s="1">
+        <v>43845.5</v>
+      </c>
+      <c r="B661">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="662" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A662" s="1">
+        <v>43846.5</v>
+      </c>
+      <c r="B662">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="663" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A663" s="1">
+        <v>43847.5</v>
+      </c>
+      <c r="B663">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="664" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A664" s="1">
+        <v>43848.5</v>
+      </c>
+      <c r="B664">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="665" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A665" s="1">
+        <v>43849.5</v>
+      </c>
+      <c r="B665">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="666" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A666" s="1">
+        <v>43850.5</v>
+      </c>
+      <c r="B666">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="667" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A667" s="1">
+        <v>43851.5</v>
+      </c>
+      <c r="B667">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="668" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A668" s="1">
+        <v>43852.5</v>
+      </c>
+      <c r="B668">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="669" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A669" s="1">
+        <v>43853.5</v>
+      </c>
+      <c r="B669">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="670" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A670" s="1">
+        <v>43854.5</v>
+      </c>
+      <c r="B670">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="671" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A671" s="1">
+        <v>43855.5</v>
+      </c>
+      <c r="B671">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="672" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A672" s="1">
+        <v>43856.5</v>
+      </c>
+      <c r="B672">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="673" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A673" s="1">
+        <v>43857.5</v>
+      </c>
+      <c r="B673">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="674" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A674" s="1">
+        <v>43858.5</v>
+      </c>
+      <c r="B674">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="675" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A675" s="1">
+        <v>43859.5</v>
+      </c>
+      <c r="B675">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="676" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A676" s="1">
+        <v>43860.5</v>
+      </c>
+      <c r="B676">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="677" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A677" s="1">
+        <v>43861.5</v>
+      </c>
+      <c r="B677">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="678" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A678" s="1">
+        <v>43862.5</v>
+      </c>
+      <c r="B678">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="679" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A679" s="1">
+        <v>43863.5</v>
+      </c>
+      <c r="B679">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="680" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A680" s="1">
+        <v>43864.5</v>
+      </c>
+      <c r="B680">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="681" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A681" s="1">
+        <v>43865.5</v>
+      </c>
+      <c r="B681">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="682" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A682" s="1">
+        <v>43866.5</v>
+      </c>
+      <c r="B682">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="683" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A683" s="1">
+        <v>43867.5</v>
+      </c>
+      <c r="B683">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="684" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A684" s="1">
+        <v>43868.5</v>
+      </c>
+      <c r="B684">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="685" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A685" s="1">
+        <v>43869.5</v>
+      </c>
+      <c r="B685">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="686" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A686" s="1">
+        <v>43870.5</v>
+      </c>
+      <c r="B686">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="687" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A687" s="1">
+        <v>43871.5</v>
+      </c>
+      <c r="B687">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="688" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A688" s="1">
+        <v>43872.5</v>
+      </c>
+      <c r="B688">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="689" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A689" s="1">
+        <v>43873.5</v>
+      </c>
+      <c r="B689">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="690" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A690" s="1">
+        <v>43874.5</v>
+      </c>
+      <c r="B690">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="691" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A691" s="1">
+        <v>43875.5</v>
+      </c>
+      <c r="B691">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="692" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A692" s="1">
+        <v>43876.5</v>
+      </c>
+      <c r="B692">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="693" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A693" s="1">
+        <v>43877.5</v>
+      </c>
+      <c r="B693">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="694" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A694" s="1">
+        <v>43878.5</v>
+      </c>
+      <c r="B694">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="695" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A695" s="1">
+        <v>43879.5</v>
+      </c>
+      <c r="B695">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="696" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A696" s="1">
+        <v>43880.5</v>
+      </c>
+      <c r="B696">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="697" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A697" s="1">
+        <v>43881.5</v>
+      </c>
+      <c r="B697">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="698" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A698" s="1">
+        <v>43882.5</v>
+      </c>
+      <c r="B698">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="699" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A699" s="1">
+        <v>43883.5</v>
+      </c>
+      <c r="B699">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="700" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A700" s="1">
+        <v>43884.5</v>
+      </c>
+      <c r="B700">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="701" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A701" s="1">
+        <v>43885.5</v>
+      </c>
+      <c r="B701">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="702" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A702" s="1">
+        <v>43886.5</v>
+      </c>
+      <c r="B702">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="703" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A703" s="1">
+        <v>43887.5</v>
+      </c>
+      <c r="B703">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="704" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A704" s="1">
+        <v>43888.5</v>
+      </c>
+      <c r="B704">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="705" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A705" s="1">
+        <v>43889.5</v>
+      </c>
+      <c r="B705">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="706" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A706" s="1">
+        <v>43890.5</v>
+      </c>
+      <c r="B706">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="707" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A707" s="1">
+        <v>43891.5</v>
+      </c>
+      <c r="B707">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="708" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A708" s="1">
+        <v>43892.5</v>
+      </c>
+      <c r="B708">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="709" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A709" s="1">
+        <v>43893.5</v>
+      </c>
+      <c r="B709">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="710" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A710" s="1">
+        <v>43894.5</v>
+      </c>
+      <c r="B710">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="711" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A711" s="1">
+        <v>43895.5</v>
+      </c>
+      <c r="B711">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="712" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A712" s="1">
+        <v>43896.5</v>
+      </c>
+      <c r="B712">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="713" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A713" s="1">
+        <v>43897.5</v>
+      </c>
+      <c r="B713">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="714" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A714" s="1">
+        <v>43898.5</v>
+      </c>
+      <c r="B714">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="715" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A715" s="1">
+        <v>43899.5</v>
+      </c>
+      <c r="B715">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="716" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A716" s="1">
+        <v>43900.5</v>
+      </c>
+      <c r="B716">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="717" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A717" s="1">
+        <v>43901.5</v>
+      </c>
+      <c r="B717">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="718" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A718" s="1">
+        <v>43902.5</v>
+      </c>
+      <c r="B718">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="719" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A719" s="1">
+        <v>43903.5</v>
+      </c>
+      <c r="B719">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="720" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A720" s="1">
+        <v>43904.5</v>
+      </c>
+      <c r="B720">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="721" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A721" s="1">
+        <v>43905.5</v>
+      </c>
+      <c r="B721">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="722" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A722" s="1">
+        <v>43906.5</v>
+      </c>
+      <c r="B722">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="723" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A723" s="1">
+        <v>43907.5</v>
+      </c>
+      <c r="B723">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="724" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A724" s="1">
+        <v>43908.5</v>
+      </c>
+      <c r="B724">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="725" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A725" s="1">
+        <v>43909.5</v>
+      </c>
+      <c r="B725">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="726" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A726" s="1">
+        <v>43910.5</v>
+      </c>
+      <c r="B726">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="727" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A727" s="1">
+        <v>43911.5</v>
+      </c>
+      <c r="B727">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="728" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A728" s="1">
+        <v>43912.5</v>
+      </c>
+      <c r="B728">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="729" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A729" s="1">
+        <v>43913.5</v>
+      </c>
+      <c r="B729">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="730" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A730" s="1">
+        <v>43914.5</v>
+      </c>
+      <c r="B730">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="731" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A731" s="1">
+        <v>43915.5</v>
+      </c>
+      <c r="B731">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="732" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A732" s="1">
+        <v>43916.5</v>
+      </c>
+      <c r="B732">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="733" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A733" s="1">
+        <v>43917.5</v>
+      </c>
+      <c r="B733">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="734" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A734" s="1">
+        <v>43918.5</v>
+      </c>
+      <c r="B734">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="735" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A735" s="1">
+        <v>43919.5</v>
+      </c>
+      <c r="B735">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="736" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A736" s="1">
+        <v>43920.5</v>
+      </c>
+      <c r="B736">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="737" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A737" s="1">
+        <v>43921.5</v>
+      </c>
+      <c r="B737">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="738" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A738" s="1">
+        <v>43922.5</v>
+      </c>
+      <c r="B738">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="739" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A739" s="1">
+        <v>43923.5</v>
+      </c>
+      <c r="B739">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="740" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A740" s="1">
+        <v>43924.5</v>
+      </c>
+      <c r="B740">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="741" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A741" s="1">
+        <v>43925.5</v>
+      </c>
+      <c r="B741">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="742" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A742" s="1">
+        <v>43926.5</v>
+      </c>
+      <c r="B742">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="743" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A743" s="1">
+        <v>43927.5</v>
+      </c>
+      <c r="B743">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="744" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A744" s="1">
+        <v>43928.5</v>
+      </c>
+      <c r="B744">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="745" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A745" s="1">
+        <v>43929.5</v>
+      </c>
+      <c r="B745">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="746" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A746" s="1">
+        <v>43930.5</v>
+      </c>
+      <c r="B746">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="747" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A747" s="1">
+        <v>43931.5</v>
+      </c>
+      <c r="B747">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="748" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A748" s="1">
+        <v>43932.5</v>
+      </c>
+      <c r="B748">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="749" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A749" s="1">
+        <v>43933.5</v>
+      </c>
+      <c r="B749">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="750" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A750" s="1">
+        <v>43934.5</v>
+      </c>
+      <c r="B750">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="751" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A751" s="1">
+        <v>43935.5</v>
+      </c>
+      <c r="B751">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="752" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A752" s="1">
+        <v>43936.5</v>
+      </c>
+      <c r="B752">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="753" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A753" s="1">
+        <v>43937.5</v>
+      </c>
+      <c r="B753">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="754" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A754" s="1">
+        <v>43938.5</v>
+      </c>
+      <c r="B754">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="755" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A755" s="1">
+        <v>43939.5</v>
+      </c>
+      <c r="B755">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="756" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A756" s="1">
+        <v>43940.5</v>
+      </c>
+      <c r="B756">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="757" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A757" s="1">
+        <v>43941.5</v>
+      </c>
+      <c r="B757">
+        <v>309</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>